<commit_message>
WIP on better calibration
</commit_message>
<xml_diff>
--- a/scan2000_calibrate/results.xlsx
+++ b/scan2000_calibrate/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hboot/Documents/personal/bricolage/HomeProjects/scannercard/SCAN2000_breakout/scan2000_calibrate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15113835-8373-EE45-9E7D-C5B1E49F455D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906F198E-CEA5-FF4D-83E7-5F12107C0BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1500" windowWidth="33480" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4003,8 +4003,8 @@
         <c:axId val="1522158912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="10.1"/>
-          <c:min val="9.9499999999999993"/>
+          <c:max val="10.07"/>
+          <c:min val="9.9700000000000006"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -7534,8 +7534,8 @@
         <c:axId val="1519588352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="10.1"/>
-          <c:min val="9.9499999999999993"/>
+          <c:max val="10.07"/>
+          <c:min val="9.9700000000000006"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -14919,7 +14919,7 @@
   <dimension ref="A1:N261"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="M2" sqref="M2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>